<commit_message>
[WBCAMS-375] Update CT dataset, v2
</commit_message>
<xml_diff>
--- a/migration/data/WorkBC_Career_Trek_2023__Apr17_24.xlsx
+++ b/migration/data/WorkBC_Career_Trek_2023__Apr17_24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CEU\7. WORKBC and PROJECTS\LMI Data Updates\2023-24\2023 LMO\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AF960FA-11FB-49E7-860D-94F2401AA030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{06FD4989-9D0A-4AF3-A34D-DBAB0C2D0918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="86280" yWindow="8055" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="1439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="1438">
   <si>
     <t>NOC 2016</t>
   </si>
@@ -3484,9 +3484,6 @@
   </si>
   <si>
     <t>East Vancouver</t>
-  </si>
-  <si>
-    <t>Lower Mainland/Southwest</t>
   </si>
   <si>
     <t>Northeast</t>
@@ -5005,8 +5002,8 @@
   <dimension ref="A1:J193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E166" sqref="E166"/>
+      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I186" sqref="I186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5067,7 +5064,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>9</v>
@@ -5082,10 +5079,10 @@
         <v>1105</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5114,10 +5111,10 @@
         <v>1105</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5131,7 +5128,7 @@
         <v>21</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>22</v>
@@ -5146,10 +5143,10 @@
         <v>1112</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5163,7 +5160,7 @@
         <v>27</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>28</v>
@@ -5178,10 +5175,10 @@
         <v>1105</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J5" s="19" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5195,7 +5192,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>28</v>
@@ -5210,10 +5207,10 @@
         <v>1105</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5242,10 +5239,10 @@
         <v>1105</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="78" x14ac:dyDescent="0.35">
@@ -5259,7 +5256,7 @@
         <v>182</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>134</v>
@@ -5274,10 +5271,10 @@
         <v>1105</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5291,7 +5288,7 @@
         <v>494</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>495</v>
@@ -5306,10 +5303,10 @@
         <v>1118</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5338,10 +5335,10 @@
         <v>1137</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5355,7 +5352,7 @@
         <v>624</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>625</v>
@@ -5370,10 +5367,10 @@
         <v>1105</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5402,10 +5399,10 @@
         <v>1105</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5419,7 +5416,7 @@
         <v>720</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>721</v>
@@ -5434,10 +5431,10 @@
         <v>1123</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5451,7 +5448,7 @@
         <v>726</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>727</v>
@@ -5466,10 +5463,10 @@
         <v>1118</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5498,10 +5495,10 @@
         <v>1118</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J15" s="19" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -5515,7 +5512,7 @@
         <v>839</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>840</v>
@@ -5530,10 +5527,10 @@
         <v>1136</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5547,7 +5544,7 @@
         <v>845</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>846</v>
@@ -5562,10 +5559,10 @@
         <v>1133</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5579,7 +5576,7 @@
         <v>1001</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>1002</v>
@@ -5594,10 +5591,10 @@
         <v>1109</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5611,7 +5608,7 @@
         <v>1007</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>1008</v>
@@ -5626,10 +5623,10 @@
         <v>1121</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5658,10 +5655,10 @@
         <v>1134</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J20" s="19" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5675,7 +5672,7 @@
         <v>36</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>37</v>
@@ -5690,10 +5687,10 @@
         <v>1116</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5722,10 +5719,10 @@
         <v>1105</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J22" s="19" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5739,7 +5736,7 @@
         <v>49</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>50</v>
@@ -5754,10 +5751,10 @@
         <v>1125</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="39" x14ac:dyDescent="0.35">
@@ -5786,10 +5783,10 @@
         <v>1105</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J24" s="19" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5818,10 +5815,10 @@
         <v>1105</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5850,10 +5847,10 @@
         <v>1105</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J26" s="19" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5867,7 +5864,7 @@
         <v>605</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>606</v>
@@ -5882,10 +5879,10 @@
         <v>1105</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J27" s="19" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -5914,10 +5911,10 @@
         <v>1105</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J28" s="19" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -5946,10 +5943,10 @@
         <v>1144</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5963,7 +5960,7 @@
         <v>69</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>70</v>
@@ -5978,10 +5975,10 @@
         <v>1111</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="J30" s="19" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -5995,7 +5992,7 @@
         <v>96</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>97</v>
@@ -6010,10 +6007,10 @@
         <v>1105</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J31" s="19" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6042,10 +6039,10 @@
         <v>1110</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6074,10 +6071,10 @@
         <v>1105</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J33" s="19" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6091,7 +6088,7 @@
         <v>115</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>116</v>
@@ -6106,10 +6103,10 @@
         <v>1125</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J34" s="19" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -6123,7 +6120,7 @@
         <v>982</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>983</v>
@@ -6138,10 +6135,10 @@
         <v>1105</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J35" s="19" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6155,7 +6152,7 @@
         <v>121</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>122</v>
@@ -6170,10 +6167,10 @@
         <v>1107</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J36" s="19" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6202,10 +6199,10 @@
         <v>1105</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J37" s="19" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6219,7 +6216,7 @@
         <v>143</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>144</v>
@@ -6234,10 +6231,10 @@
         <v>1105</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J38" s="19" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6251,7 +6248,7 @@
         <v>149</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>150</v>
@@ -6266,10 +6263,10 @@
         <v>1122</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J39" s="19" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6298,10 +6295,10 @@
         <v>1112</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="J40" s="19" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -6330,10 +6327,10 @@
         <v>1128</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J41" s="19" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="78" x14ac:dyDescent="0.35">
@@ -6362,10 +6359,10 @@
         <v>1125</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J42" s="19" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6394,10 +6391,10 @@
         <v>1142</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J43" s="20" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6411,7 +6408,7 @@
         <v>235</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>236</v>
@@ -6426,10 +6423,10 @@
         <v>1105</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J44" s="19" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6458,10 +6455,10 @@
         <v>1125</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J45" s="19" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6490,10 +6487,10 @@
         <v>1105</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="J46" s="19" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6507,7 +6504,7 @@
         <v>179</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>180</v>
@@ -6522,10 +6519,10 @@
         <v>1117</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J47" s="19" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6554,10 +6551,10 @@
         <v>1110</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="J48" s="19" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="78" x14ac:dyDescent="0.35">
@@ -6571,7 +6568,7 @@
         <v>192</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>193</v>
@@ -6586,10 +6583,10 @@
         <v>1128</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J49" s="19" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -6603,7 +6600,7 @@
         <v>198</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>199</v>
@@ -6618,10 +6615,10 @@
         <v>1106</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J50" s="19" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6635,7 +6632,7 @@
         <v>204</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>205</v>
@@ -6650,10 +6647,10 @@
         <v>1125</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J51" s="19" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6682,10 +6679,10 @@
         <v>1105</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="J52" s="19" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6714,10 +6711,10 @@
         <v>1105</v>
       </c>
       <c r="I53" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J53" s="19" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="78" x14ac:dyDescent="0.35">
@@ -6746,10 +6743,10 @@
         <v>1125</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J54" s="19" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -6763,7 +6760,7 @@
         <v>241</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>242</v>
@@ -6778,10 +6775,10 @@
         <v>1135</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J55" s="19" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -6795,7 +6792,7 @@
         <v>247</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>248</v>
@@ -6810,10 +6807,10 @@
         <v>1109</v>
       </c>
       <c r="I56" s="11" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="J56" s="19" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6827,7 +6824,7 @@
         <v>253</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>254</v>
@@ -6842,10 +6839,10 @@
         <v>1135</v>
       </c>
       <c r="I57" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J57" s="19" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -6859,7 +6856,7 @@
         <v>259</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>260</v>
@@ -6874,10 +6871,10 @@
         <v>1125</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J58" s="19" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6906,10 +6903,10 @@
         <v>1106</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J59" s="19" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -6938,10 +6935,10 @@
         <v>1105</v>
       </c>
       <c r="I60" s="11" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="J60" s="19" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -6955,7 +6952,7 @@
         <v>312</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>313</v>
@@ -6970,10 +6967,10 @@
         <v>1129</v>
       </c>
       <c r="I61" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J61" s="19" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -6987,7 +6984,7 @@
         <v>265</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>266</v>
@@ -7002,10 +6999,10 @@
         <v>1114</v>
       </c>
       <c r="I62" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J62" s="19" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="58" customHeight="1" x14ac:dyDescent="0.35">
@@ -7019,7 +7016,7 @@
         <v>285</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>286</v>
@@ -7034,10 +7031,10 @@
         <v>1105</v>
       </c>
       <c r="I63" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J63" s="19" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -7066,10 +7063,10 @@
         <v>1109</v>
       </c>
       <c r="I64" s="11" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="J64" s="19" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7083,7 +7080,7 @@
         <v>937</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>938</v>
@@ -7098,10 +7095,10 @@
         <v>1105</v>
       </c>
       <c r="I65" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J65" s="19" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7130,10 +7127,10 @@
         <v>1111</v>
       </c>
       <c r="I66" s="11" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="J66" s="19" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7147,7 +7144,7 @@
         <v>950</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>951</v>
@@ -7162,10 +7159,10 @@
         <v>1111</v>
       </c>
       <c r="I67" s="11" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="J67" s="19" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7194,10 +7191,10 @@
         <v>1140</v>
       </c>
       <c r="I68" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J68" s="19" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7226,10 +7223,10 @@
         <v>1123</v>
       </c>
       <c r="I69" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J69" s="19" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7243,7 +7240,7 @@
         <v>395</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>396</v>
@@ -7258,10 +7255,10 @@
         <v>1124</v>
       </c>
       <c r="I70" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J70" s="19" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7290,10 +7287,10 @@
         <v>1114</v>
       </c>
       <c r="I71" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J71" s="19" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7307,7 +7304,7 @@
         <v>325</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>326</v>
@@ -7322,10 +7319,10 @@
         <v>1125</v>
       </c>
       <c r="I72" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J72" s="19" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7354,10 +7351,10 @@
         <v>1105</v>
       </c>
       <c r="I73" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J73" s="19" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="78" x14ac:dyDescent="0.35">
@@ -7386,10 +7383,10 @@
         <v>1106</v>
       </c>
       <c r="I74" s="11" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="J74" s="19" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7418,10 +7415,10 @@
         <v>1114</v>
       </c>
       <c r="I75" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J75" s="19" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7450,10 +7447,10 @@
         <v>1105</v>
       </c>
       <c r="I76" s="12" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J76" s="20" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7482,10 +7479,10 @@
         <v>1105</v>
       </c>
       <c r="I77" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J77" s="19" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7514,10 +7511,10 @@
         <v>1139</v>
       </c>
       <c r="I78" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J78" s="19" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7546,10 +7543,10 @@
         <v>1124</v>
       </c>
       <c r="I79" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J79" s="19" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7563,7 +7560,7 @@
         <v>361</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>362</v>
@@ -7578,10 +7575,10 @@
         <v>1114</v>
       </c>
       <c r="I80" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J80" s="19" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -7595,7 +7592,7 @@
         <v>365</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>362</v>
@@ -7610,10 +7607,10 @@
         <v>1106</v>
       </c>
       <c r="I81" s="11" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="J81" s="19" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="91" x14ac:dyDescent="0.35">
@@ -7627,7 +7624,7 @@
         <v>349</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>350</v>
@@ -7642,10 +7639,10 @@
         <v>1105</v>
       </c>
       <c r="I82" s="11" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="J82" s="19" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -7674,10 +7671,10 @@
         <v>1120</v>
       </c>
       <c r="I83" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J83" s="19" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7706,10 +7703,10 @@
         <v>1125</v>
       </c>
       <c r="I84" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J84" s="19" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7738,10 +7735,10 @@
         <v>1109</v>
       </c>
       <c r="I85" s="11" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="J85" s="19" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7770,10 +7767,10 @@
         <v>1114</v>
       </c>
       <c r="I86" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J86" s="19" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7787,7 +7784,7 @@
         <v>439</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>440</v>
@@ -7802,10 +7799,10 @@
         <v>1127</v>
       </c>
       <c r="I87" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J87" s="19" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7819,7 +7816,7 @@
         <v>433</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>434</v>
@@ -7834,10 +7831,10 @@
         <v>1105</v>
       </c>
       <c r="I88" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J88" s="19" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7866,10 +7863,10 @@
         <v>1118</v>
       </c>
       <c r="I89" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J89" s="19" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7883,7 +7880,7 @@
         <v>445</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>446</v>
@@ -7898,10 +7895,10 @@
         <v>1119</v>
       </c>
       <c r="I90" s="11" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="J90" s="19" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7930,10 +7927,10 @@
         <v>1125</v>
       </c>
       <c r="I91" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J91" s="19" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7962,10 +7959,10 @@
         <v>1146</v>
       </c>
       <c r="I92" s="11" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="J92" s="19" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -7994,10 +7991,10 @@
         <v>1105</v>
       </c>
       <c r="I93" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J93" s="19" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8026,10 +8023,10 @@
         <v>1111</v>
       </c>
       <c r="I94" s="11" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="J94" s="19" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8058,10 +8055,10 @@
         <v>1117</v>
       </c>
       <c r="I95" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J95" s="19" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8090,10 +8087,10 @@
         <v>1119</v>
       </c>
       <c r="I96" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J96" s="19" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="97" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -8107,7 +8104,7 @@
         <v>488</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="E97" s="6" t="s">
         <v>489</v>
@@ -8122,10 +8119,10 @@
         <v>1105</v>
       </c>
       <c r="I97" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J97" s="19" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="98" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8139,7 +8136,7 @@
         <v>513</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="E98" s="6" t="s">
         <v>514</v>
@@ -8154,10 +8151,10 @@
         <v>1105</v>
       </c>
       <c r="I98" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J98" s="19" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="99" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -8171,7 +8168,7 @@
         <v>519</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="E99" s="6" t="s">
         <v>520</v>
@@ -8186,10 +8183,10 @@
         <v>1114</v>
       </c>
       <c r="I99" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J99" s="19" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -8203,7 +8200,7 @@
         <v>179</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>525</v>
@@ -8218,10 +8215,10 @@
         <v>1125</v>
       </c>
       <c r="I100" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J100" s="19" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="101" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8235,7 +8232,7 @@
         <v>507</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="E101" s="6" t="s">
         <v>508</v>
@@ -8250,10 +8247,10 @@
         <v>1125</v>
       </c>
       <c r="I101" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J101" s="19" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="102" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8282,10 +8279,10 @@
         <v>1123</v>
       </c>
       <c r="I102" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J102" s="19" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="103" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8314,10 +8311,10 @@
         <v>1116</v>
       </c>
       <c r="I103" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J103" s="19" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="78" x14ac:dyDescent="0.35">
@@ -8346,10 +8343,10 @@
         <v>1123</v>
       </c>
       <c r="I104" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J104" s="19" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="105" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8363,7 +8360,7 @@
         <v>537</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="E105" s="6" t="s">
         <v>538</v>
@@ -8378,10 +8375,10 @@
         <v>1125</v>
       </c>
       <c r="I105" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J105" s="19" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="106" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8410,10 +8407,10 @@
         <v>1116</v>
       </c>
       <c r="I106" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J106" s="19" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="107" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8427,7 +8424,7 @@
         <v>550</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="E107" s="6" t="s">
         <v>551</v>
@@ -8442,10 +8439,10 @@
         <v>1123</v>
       </c>
       <c r="I107" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J107" s="19" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="108" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8459,7 +8456,7 @@
         <v>556</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>557</v>
@@ -8474,10 +8471,10 @@
         <v>1105</v>
       </c>
       <c r="I108" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J108" s="19" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="109" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -8491,7 +8488,7 @@
         <v>562</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="E109" s="6" t="s">
         <v>563</v>
@@ -8506,10 +8503,10 @@
         <v>1105</v>
       </c>
       <c r="I109" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J109" s="19" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="110" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8523,7 +8520,7 @@
         <v>154</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="E110" s="6" t="s">
         <v>150</v>
@@ -8538,10 +8535,10 @@
         <v>1105</v>
       </c>
       <c r="I110" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J110" s="19" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="111" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8555,7 +8552,7 @@
         <v>581</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="E111" s="6" t="s">
         <v>582</v>
@@ -8570,10 +8567,10 @@
         <v>1125</v>
       </c>
       <c r="I111" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J111" s="19" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="112" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8587,7 +8584,7 @@
         <v>587</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="E112" s="6" t="s">
         <v>588</v>
@@ -8602,10 +8599,10 @@
         <v>1138</v>
       </c>
       <c r="I112" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J112" s="19" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="113" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8619,7 +8616,7 @@
         <v>593</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="E113" s="6" t="s">
         <v>594</v>
@@ -8634,10 +8631,10 @@
         <v>1113</v>
       </c>
       <c r="I113" s="11" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="J113" s="19" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="114" spans="1:10" s="1" customFormat="1" ht="91" x14ac:dyDescent="0.35">
@@ -8666,10 +8663,10 @@
         <v>1118</v>
       </c>
       <c r="I114" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J114" s="19" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8698,10 +8695,10 @@
         <v>1125</v>
       </c>
       <c r="I115" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J115" s="19" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="116" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8730,10 +8727,10 @@
         <v>1110</v>
       </c>
       <c r="I116" s="11" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="J116" s="19" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8762,10 +8759,10 @@
         <v>1105</v>
       </c>
       <c r="I117" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J117" s="19" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8779,7 +8776,7 @@
         <v>618</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="E118" s="6" t="s">
         <v>619</v>
@@ -8794,10 +8791,10 @@
         <v>1122</v>
       </c>
       <c r="I118" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J118" s="19" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="119" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -8811,7 +8808,7 @@
         <v>599</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="E119" s="6" t="s">
         <v>600</v>
@@ -8826,10 +8823,10 @@
         <v>1105</v>
       </c>
       <c r="I119" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J119" s="19" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="120" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8858,10 +8855,10 @@
         <v>1123</v>
       </c>
       <c r="I120" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J120" s="19" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="121" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8875,7 +8872,7 @@
         <v>642</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="E121" s="6" t="s">
         <v>643</v>
@@ -8890,10 +8887,10 @@
         <v>1118</v>
       </c>
       <c r="I121" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J121" s="19" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="122" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8922,10 +8919,10 @@
         <v>1109</v>
       </c>
       <c r="I122" s="11" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="J122" s="19" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="123" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8954,10 +8951,10 @@
         <v>1123</v>
       </c>
       <c r="I123" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J123" s="19" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="124" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -8971,7 +8968,7 @@
         <v>654</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="E124" s="6" t="s">
         <v>655</v>
@@ -8986,10 +8983,10 @@
         <v>1105</v>
       </c>
       <c r="I124" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J124" s="19" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="125" spans="1:10" ht="78" x14ac:dyDescent="0.35">
@@ -9018,10 +9015,10 @@
         <v>1118</v>
       </c>
       <c r="I125" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J125" s="19" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="126" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9035,7 +9032,7 @@
         <v>660</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="E126" s="6" t="s">
         <v>661</v>
@@ -9050,10 +9047,10 @@
         <v>1105</v>
       </c>
       <c r="I126" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J126" s="19" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="127" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9067,7 +9064,7 @@
         <v>666</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="E127" s="6" t="s">
         <v>667</v>
@@ -9082,10 +9079,10 @@
         <v>1114</v>
       </c>
       <c r="I127" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J127" s="19" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="128" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
@@ -9099,7 +9096,7 @@
         <v>672</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="E128" s="6" t="s">
         <v>673</v>
@@ -9114,10 +9111,10 @@
         <v>1136</v>
       </c>
       <c r="I128" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J128" s="19" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="129" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9131,7 +9128,7 @@
         <v>696</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="E129" s="6" t="s">
         <v>697</v>
@@ -9146,10 +9143,10 @@
         <v>1105</v>
       </c>
       <c r="I129" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J129" s="19" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="130" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9163,7 +9160,7 @@
         <v>678</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="E130" s="6" t="s">
         <v>679</v>
@@ -9178,10 +9175,10 @@
         <v>1120</v>
       </c>
       <c r="I130" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J130" s="19" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="131" spans="1:10" ht="78" x14ac:dyDescent="0.35">
@@ -9210,10 +9207,10 @@
         <v>1105</v>
       </c>
       <c r="I131" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J131" s="20" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="132" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -9227,7 +9224,7 @@
         <v>702</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="E132" s="6" t="s">
         <v>703</v>
@@ -9242,10 +9239,10 @@
         <v>1105</v>
       </c>
       <c r="I132" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J132" s="19" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="133" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9259,7 +9256,7 @@
         <v>708</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="E133" s="6" t="s">
         <v>709</v>
@@ -9274,10 +9271,10 @@
         <v>1114</v>
       </c>
       <c r="I133" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J133" s="19" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="134" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -9306,10 +9303,10 @@
         <v>1118</v>
       </c>
       <c r="I134" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J134" s="19" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="135" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9338,10 +9335,10 @@
         <v>1143</v>
       </c>
       <c r="I135" s="12" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J135" s="19" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="136" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9355,7 +9352,7 @@
         <v>759</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="E136" s="6" t="s">
         <v>760</v>
@@ -9370,10 +9367,10 @@
         <v>1123</v>
       </c>
       <c r="I136" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J136" s="19" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="137" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9387,7 +9384,7 @@
         <v>765</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="E137" s="6" t="s">
         <v>766</v>
@@ -9402,10 +9399,10 @@
         <v>1118</v>
       </c>
       <c r="I137" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J137" s="19" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="138" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9434,10 +9431,10 @@
         <v>1105</v>
       </c>
       <c r="I138" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J138" s="19" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="139" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9466,10 +9463,10 @@
         <v>1114</v>
       </c>
       <c r="I139" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J139" s="19" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="140" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9498,10 +9495,10 @@
         <v>1118</v>
       </c>
       <c r="I140" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J140" s="19" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="141" spans="1:10" s="7" customFormat="1" ht="65" x14ac:dyDescent="0.35">
@@ -9530,10 +9527,10 @@
         <v>1125</v>
       </c>
       <c r="I141" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J141" s="19" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="142" spans="1:10" s="7" customFormat="1" ht="65" x14ac:dyDescent="0.35">
@@ -9547,7 +9544,7 @@
         <v>783</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="E142" s="6" t="s">
         <v>784</v>
@@ -9562,10 +9559,10 @@
         <v>1116</v>
       </c>
       <c r="I142" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J142" s="19" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="143" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9594,10 +9591,10 @@
         <v>1126</v>
       </c>
       <c r="I143" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J143" s="19" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="144" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9611,7 +9608,7 @@
         <v>795</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="E144" s="6" t="s">
         <v>796</v>
@@ -9626,10 +9623,10 @@
         <v>1131</v>
       </c>
       <c r="I144" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J144" s="19" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="145" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9643,7 +9640,7 @@
         <v>177</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="E145" s="6" t="s">
         <v>796</v>
@@ -9658,10 +9655,10 @@
         <v>1125</v>
       </c>
       <c r="I145" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J145" s="19" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="146" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9675,7 +9672,7 @@
         <v>815</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E146" s="6" t="s">
         <v>816</v>
@@ -9690,10 +9687,10 @@
         <v>1105</v>
       </c>
       <c r="I146" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J146" s="19" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="147" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9722,10 +9719,10 @@
         <v>1123</v>
       </c>
       <c r="I147" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J147" s="19" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="148" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9739,7 +9736,7 @@
         <v>826</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="E148" s="6" t="s">
         <v>827</v>
@@ -9754,10 +9751,10 @@
         <v>1125</v>
       </c>
       <c r="I148" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J148" s="19" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="149" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -9771,7 +9768,7 @@
         <v>820</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="E149" s="6" t="s">
         <v>821</v>
@@ -9786,10 +9783,10 @@
         <v>1125</v>
       </c>
       <c r="I149" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J149" s="19" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="150" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -9803,7 +9800,7 @@
         <v>802</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="E150" s="6" t="s">
         <v>803</v>
@@ -9818,10 +9815,10 @@
         <v>1141</v>
       </c>
       <c r="I150" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J150" s="19" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="151" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -9835,7 +9832,7 @@
         <v>851</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="E151" s="6" t="s">
         <v>852</v>
@@ -9850,10 +9847,10 @@
         <v>1125</v>
       </c>
       <c r="I151" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J151" s="19" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="152" spans="1:10" ht="78" x14ac:dyDescent="0.35">
@@ -9882,10 +9879,10 @@
         <v>1145</v>
       </c>
       <c r="I152" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J152" s="19" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="153" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -9914,10 +9911,10 @@
         <v>1125</v>
       </c>
       <c r="I153" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J153" s="19" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="154" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9931,7 +9928,7 @@
         <v>869</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="E154" s="6" t="s">
         <v>870</v>
@@ -9946,10 +9943,10 @@
         <v>1112</v>
       </c>
       <c r="I154" s="11" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="J154" s="19" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="155" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -9963,7 +9960,7 @@
         <v>875</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="E155" s="6" t="s">
         <v>876</v>
@@ -9978,10 +9975,10 @@
         <v>1116</v>
       </c>
       <c r="I155" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J155" s="19" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="156" spans="1:10" ht="78" x14ac:dyDescent="0.35">
@@ -9995,7 +9992,7 @@
         <v>184</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="E156" s="6" t="s">
         <v>876</v>
@@ -10010,10 +10007,10 @@
         <v>1118</v>
       </c>
       <c r="I156" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J156" s="19" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="157" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -10042,10 +10039,10 @@
         <v>1105</v>
       </c>
       <c r="I157" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J157" s="19" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="158" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -10059,7 +10056,7 @@
         <v>887</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="E158" s="6" t="s">
         <v>888</v>
@@ -10074,10 +10071,10 @@
         <v>1125</v>
       </c>
       <c r="I158" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J158" s="19" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="159" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -10106,10 +10103,10 @@
         <v>1112</v>
       </c>
       <c r="I159" s="11" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="J159" s="19" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="160" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10138,10 +10135,10 @@
         <v>1114</v>
       </c>
       <c r="I160" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J160" s="19" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="161" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10155,7 +10152,7 @@
         <v>905</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="E161" s="6" t="s">
         <v>906</v>
@@ -10170,10 +10167,10 @@
         <v>1118</v>
       </c>
       <c r="I161" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J161" s="19" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="162" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10202,10 +10199,10 @@
         <v>1131</v>
       </c>
       <c r="I162" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J162" s="19" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="163" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10219,7 +10216,7 @@
         <v>918</v>
       </c>
       <c r="D163" s="6" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="E163" s="6" t="s">
         <v>919</v>
@@ -10234,10 +10231,10 @@
         <v>1130</v>
       </c>
       <c r="I163" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J163" s="19" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="164" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -10251,7 +10248,7 @@
         <v>924</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="E164" s="6" t="s">
         <v>925</v>
@@ -10266,10 +10263,10 @@
         <v>1105</v>
       </c>
       <c r="I164" s="11" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="J164" s="19" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="165" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10283,7 +10280,7 @@
         <v>930</v>
       </c>
       <c r="D165" s="6" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="E165" s="6" t="s">
         <v>931</v>
@@ -10298,10 +10295,10 @@
         <v>1109</v>
       </c>
       <c r="I165" s="11" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="J165" s="19" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="166" spans="1:10" ht="117" x14ac:dyDescent="0.35">
@@ -10315,7 +10312,7 @@
         <v>175</v>
       </c>
       <c r="D166" s="6" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="E166" s="6" t="s">
         <v>931</v>
@@ -10324,16 +10321,16 @@
         <v>934</v>
       </c>
       <c r="G166" s="22" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="H166" s="11" t="s">
         <v>1123</v>
       </c>
       <c r="I166" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J166" s="19" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="167" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10347,7 +10344,7 @@
         <v>969</v>
       </c>
       <c r="D167" s="6" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="E167" s="6" t="s">
         <v>970</v>
@@ -10362,10 +10359,10 @@
         <v>1137</v>
       </c>
       <c r="I167" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J167" s="19" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="168" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10394,10 +10391,10 @@
         <v>1111</v>
       </c>
       <c r="I168" s="11" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="J168" s="19" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="169" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10426,10 +10423,10 @@
         <v>1112</v>
       </c>
       <c r="I169" s="11" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="J169" s="19" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="170" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10443,7 +10440,7 @@
         <v>963</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="E170" s="6" t="s">
         <v>964</v>
@@ -10458,10 +10455,10 @@
         <v>1105</v>
       </c>
       <c r="I170" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J170" s="19" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="171" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10490,10 +10487,10 @@
         <v>1110</v>
       </c>
       <c r="I171" s="11" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="J171" s="19" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="172" spans="1:10" ht="78" x14ac:dyDescent="0.35">
@@ -10516,16 +10513,16 @@
         <v>978</v>
       </c>
       <c r="G172" s="16" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="H172" s="11" t="s">
         <v>1123</v>
       </c>
       <c r="I172" s="11" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J172" s="19" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="173" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10539,7 +10536,7 @@
         <v>988</v>
       </c>
       <c r="D173" s="6" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="E173" s="6" t="s">
         <v>989</v>
@@ -10554,10 +10551,10 @@
         <v>1111</v>
       </c>
       <c r="I173" s="11" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="J173" s="19" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="174" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10571,7 +10568,7 @@
         <v>1013</v>
       </c>
       <c r="D174" s="6" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="E174" s="6" t="s">
         <v>1014</v>
@@ -10586,10 +10583,10 @@
         <v>1109</v>
       </c>
       <c r="I174" s="11" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="J174" s="19" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="175" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10603,7 +10600,7 @@
         <v>1019</v>
       </c>
       <c r="D175" s="6" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="E175" s="6" t="s">
         <v>1020</v>
@@ -10618,10 +10615,10 @@
         <v>1132</v>
       </c>
       <c r="I175" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J175" s="19" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="176" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10650,10 +10647,10 @@
         <v>1105</v>
       </c>
       <c r="I176" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J176" s="19" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="177" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10667,7 +10664,7 @@
         <v>1032</v>
       </c>
       <c r="D177" s="6" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="E177" s="6" t="s">
         <v>1033</v>
@@ -10682,10 +10679,10 @@
         <v>1117</v>
       </c>
       <c r="I177" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J177" s="19" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="178" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -10699,7 +10696,7 @@
         <v>1045</v>
       </c>
       <c r="D178" s="6" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="E178" s="6" t="s">
         <v>1046</v>
@@ -10714,10 +10711,10 @@
         <v>1129</v>
       </c>
       <c r="I178" s="11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="J178" s="19" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="179" spans="1:10" ht="52" x14ac:dyDescent="0.35">
@@ -10731,7 +10728,7 @@
         <v>1051</v>
       </c>
       <c r="D179" s="6" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="E179" s="6" t="s">
         <v>1052</v>
@@ -10746,10 +10743,10 @@
         <v>1117</v>
       </c>
       <c r="I179" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J179" s="19" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="180" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10778,10 +10775,10 @@
         <v>1120</v>
       </c>
       <c r="I180" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J180" s="19" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="181" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10810,10 +10807,10 @@
         <v>1115</v>
       </c>
       <c r="I181" s="11" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J181" s="19" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="182" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10827,7 +10824,7 @@
         <v>1077</v>
       </c>
       <c r="D182" s="6" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="E182" s="6" t="s">
         <v>1078</v>
@@ -10842,10 +10839,10 @@
         <v>1134</v>
       </c>
       <c r="I182" s="11" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J182" s="19" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="183" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10859,7 +10856,7 @@
         <v>1071</v>
       </c>
       <c r="D183" s="6" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="E183" s="6" t="s">
         <v>1072</v>
@@ -10874,10 +10871,10 @@
         <v>1105</v>
       </c>
       <c r="I183" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J183" s="19" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="184" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10891,7 +10888,7 @@
         <v>1083</v>
       </c>
       <c r="D184" s="6" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="E184" s="6" t="s">
         <v>1084</v>
@@ -10906,10 +10903,10 @@
         <v>1113</v>
       </c>
       <c r="I184" s="11" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="J184" s="19" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="185" spans="1:10" ht="65" x14ac:dyDescent="0.35">
@@ -10923,7 +10920,7 @@
         <v>1089</v>
       </c>
       <c r="D185" s="6" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="E185" s="6" t="s">
         <v>1090</v>
@@ -10938,10 +10935,10 @@
         <v>1108</v>
       </c>
       <c r="I185" s="11" t="s">
-        <v>1147</v>
+        <v>1154</v>
       </c>
       <c r="J185" s="19" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>